<commit_message>
modificaciones a carpeta 09 y 04: alvaro
</commit_message>
<xml_diff>
--- a/tspi/src/resources/notebook/02. Summary/Schedule Planning SCHEDULE.xlsx
+++ b/tspi/src/resources/notebook/02. Summary/Schedule Planning SCHEDULE.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="22600" windowHeight="13560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -78,8 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,23 +274,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
@@ -300,16 +300,16 @@
     </border>
     <border>
       <left style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -337,112 +337,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -458,6 +352,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +544,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="DFDFDF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -857,237 +857,237 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.375" customWidth="1"/>
-    <col min="10" max="10" width="3.625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.33203125" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:12" ht="16">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A3" s="36" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="3" spans="1:12" ht="16" thickBot="1">
+      <c r="A3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="36" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="41">
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="17">
         <v>42087</v>
       </c>
-      <c r="L3" s="41"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A4" s="36" t="s">
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" thickBot="1">
+      <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="36" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="37" t="s">
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="37"/>
-    </row>
-    <row r="5" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A5" s="36" t="s">
+      <c r="L4" s="18"/>
+    </row>
+    <row r="5" spans="1:12" ht="16" thickBot="1">
+      <c r="A5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="36" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="37">
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="18">
         <v>1</v>
       </c>
-      <c r="L5" s="37"/>
-    </row>
-    <row r="6" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.5" thickBot="1">
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" thickBot="1">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="27" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="29"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="18"/>
-      <c r="I8" s="7" t="s">
+      <c r="H8" s="44"/>
+      <c r="I8" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="7" t="s">
+      <c r="K8" s="44"/>
+      <c r="L8" s="37" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="15"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="8"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="15"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="8"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="38"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="15"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="8"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A13" s="16"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" ht="16.5" thickBot="1">
+      <c r="A12" s="41"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="38"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" thickBot="1">
+      <c r="A13" s="42"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="39"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="31">
         <v>42091</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="3">
         <v>25</v>
       </c>
@@ -1099,21 +1099,21 @@
         <f>D14*100/D$27</f>
         <v>7.6923076923076925</v>
       </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="34"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="16.5" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="31">
         <v>42098</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="3">
         <v>25</v>
       </c>
@@ -1125,21 +1125,21 @@
         <f>(D15*100/D$27)+F14</f>
         <v>15.384615384615385</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="13"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="34"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="16.5" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="31">
         <v>42105</v>
       </c>
-      <c r="C16" s="11"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="3">
         <v>25</v>
       </c>
@@ -1151,21 +1151,21 @@
         <f t="shared" ref="F16:F26" si="1">(D16*100/D$27)+F15</f>
         <v>23.076923076923077</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="13"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="16.5" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="31">
         <v>42112</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="3">
         <v>25</v>
       </c>
@@ -1177,21 +1177,21 @@
         <f t="shared" si="1"/>
         <v>30.76923076923077</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="34"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5" thickBot="1">
+    <row r="18" spans="1:12" ht="16" thickBot="1">
       <c r="A18" s="4">
         <v>5</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="31">
         <v>42119</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="3">
         <v>25</v>
       </c>
@@ -1203,21 +1203,21 @@
         <f t="shared" si="1"/>
         <v>38.46153846153846</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="13"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="34"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="16.5" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="4">
         <v>6</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="31">
         <v>42126</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="3">
         <v>25</v>
       </c>
@@ -1229,21 +1229,21 @@
         <f t="shared" si="1"/>
         <v>46.153846153846153</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="13"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="34"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="16.5" thickBot="1">
+    <row r="20" spans="1:12" ht="16" thickBot="1">
       <c r="A20" s="4">
         <v>7</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="31">
         <v>42133</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="3">
         <v>25</v>
       </c>
@@ -1255,25 +1255,25 @@
         <f t="shared" si="1"/>
         <v>53.846153846153847</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="13"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="16.5" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="4">
         <v>8</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="31">
         <v>42140</v>
       </c>
-      <c r="C21" s="11"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="3">
         <v>25</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="9">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
@@ -1281,25 +1281,25 @@
         <f t="shared" si="1"/>
         <v>61.53846153846154</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="13"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="16.5" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="4">
         <v>9</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="31">
         <v>42147</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="44">
+      <c r="C22" s="32"/>
+      <c r="D22" s="8">
         <v>25</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="10">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
@@ -1307,21 +1307,21 @@
         <f t="shared" si="1"/>
         <v>69.230769230769226</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="13"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" ht="16.5" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="4">
         <v>10</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="31">
         <v>42154</v>
       </c>
-      <c r="C23" s="11"/>
+      <c r="C23" s="32"/>
       <c r="D23" s="3">
         <v>25</v>
       </c>
@@ -1333,21 +1333,21 @@
         <f t="shared" si="1"/>
         <v>76.92307692307692</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="13"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" ht="16.5" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="4">
         <v>11</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="31">
         <v>42161</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="3">
         <v>25</v>
       </c>
@@ -1359,21 +1359,21 @@
         <f t="shared" si="1"/>
         <v>84.615384615384613</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="42"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="42"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="36"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" ht="16.5" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="4">
         <v>12</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="31">
         <v>42168</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="3">
         <v>25</v>
       </c>
@@ -1385,22 +1385,22 @@
         <f t="shared" si="1"/>
         <v>92.307692307692307</v>
       </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="42"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="36"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="42"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="36"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" ht="16.5" thickBot="1">
+    <row r="26" spans="1:12" ht="16" thickBot="1">
       <c r="A26" s="4">
         <v>13</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="31">
         <v>42175</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="43">
+      <c r="C26" s="32"/>
+      <c r="D26" s="7">
         <v>25</v>
       </c>
       <c r="E26" s="5">
@@ -1411,53 +1411,41 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="13"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="34"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" ht="17.25" thickTop="1" thickBot="1">
-      <c r="C27" s="47"/>
-      <c r="D27" s="48">
+    <row r="27" spans="1:12" ht="17" thickTop="1" thickBot="1">
+      <c r="C27" s="11"/>
+      <c r="D27" s="12">
         <f>SUM(D14:D26)</f>
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16.5" thickTop="1"/>
+    <row r="28" spans="1:12" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="B8:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G8:H13"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="J8:K13"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="G20:H20"/>
@@ -1474,28 +1462,39 @@
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="B8:C13"/>
     <mergeCell ref="A8:A13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="G8:H13"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="J8:K13"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>